<commit_message>
ddt-tests project updated in sync with vREST NG v2.2.8
</commit_message>
<xml_diff>
--- a/test/ddt-tests/data/create_a_new_contact.xlsx
+++ b/test/ddt-tests/data/create_a_new_contact.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44A0116-0F47-154D-95C0-71963669920F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="create_a_new_contact" state="visible" r:id="rId4"/>
+    <sheet name="create_a_new_contact" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>iterationSummary</t>
   </si>
@@ -28,9 +29,6 @@
     <t>designation</t>
   </si>
   <si>
-    <t>organization</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -49,9 +47,6 @@
     <t>Validate create API when name field is blank</t>
   </si>
   <si>
-    <t>john.doe@example.com</t>
-  </si>
-  <si>
     <t>Chief Technical Officer</t>
   </si>
   <si>
@@ -79,9 +74,6 @@
     <t>Validate create API when designation field is greater than the limit</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
     <t>Sample designation whose length is greater than the limit</t>
   </si>
   <si>
@@ -97,15 +89,6 @@
     <t>{"errors":{"organization":"field length cannot be greater than 35"}}</t>
   </si>
   <si>
-    <t>Validate create API when country field is greater than the limit</t>
-  </si>
-  <si>
-    <t>Sample country whose length is greater than the limit</t>
-  </si>
-  <si>
-    <t>{"errors":{"country":"field length cannot be greater than 35"}}</t>
-  </si>
-  <si>
     <t>Validate create API when all fields are valid</t>
   </si>
   <si>
@@ -127,35 +110,53 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>{"name":"Dheeraj Aggarwal","email":"dheeraj.aggarwal@optimizory.com","designation":"Engineering Manager","organization":"Optimizory","country":"India","aboutMe":"Passionate for making vREST NG, world's #1 API Testing Tool.","createdOn":"{{*}}","_id":"{{*}}"}</t>
+    <t>expectedName</t>
+  </si>
+  <si>
+    <t>$$skip</t>
+  </si>
+  <si>
+    <t>{{getRandom()}}</t>
+  </si>
+  <si>
+    <t>{"name":"Dheeraj Aggarwal","createdOn":"{{*}}","_id":"{{*}}","email":"dheeraj.aggarwal@optimizory.com","designation":"Engineering Manager","organization":"Optimizory","country":"India","aboutMe":"Passionate for making vREST NG, world's #1 API Testing Tool."}</t>
+  </si>
+  <si>
+    <t>{{fakeEmail}}</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>Validate create API when name field is skipped</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="16"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="16"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -499,26 +500,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="21.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="21.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
     <col min="7" max="7" width="1.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="21.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="45.33203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="21.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="57.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="21.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="43" customHeight="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -532,196 +538,217 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1">
+        <v>400</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" ht="42" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1">
+        <v>400</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1">
+    </row>
+    <row r="4" spans="1:11" ht="83" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1">
         <v>400</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
+      <c r="J4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" ht="80" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="5" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1">
+        <v>400</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="1">
         <v>400</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
+      <c r="J6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" ht="90" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1">
-        <v>400</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" ht="77" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:11" ht="169" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="1">
-        <v>400</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" ht="73" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="1">
-        <v>400</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" ht="207" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="I7" s="1">
+        <v>200</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="1">
-        <v>200</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>